<commit_message>
Use more samples for sample size calculation
</commit_message>
<xml_diff>
--- a/Unit 6/Solutions/Tradeoffs_cormorant_v_fish.xlsx
+++ b/Unit 6/Solutions/Tradeoffs_cormorant_v_fish.xlsx
@@ -1653,13 +1653,18 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ae1d7975-ef6e-42df-9d49-ebdd19403660">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100321F261CCBE9C64AB094B5E00014E60D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a8f8c1df9e84043c8e2db7d9263e1ea">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98" xmlns:ns3="ae1d7975-ef6e-42df-9d49-ebdd19403660" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="919e215a651d7e40e1a8917922009785" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100321F261CCBE9C64AB094B5E00014E60D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16f2d0d03337cb1d68bd4066c6b3dcbd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98" xmlns:ns3="ae1d7975-ef6e-42df-9d49-ebdd19403660" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="379cc4019cc3b630d26aacf100f9c3b4" ns2:_="" ns3:_="">
     <xsd:import namespace="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98"/>
     <xsd:import namespace="ae1d7975-ef6e-42df-9d49-ebdd19403660"/>
     <xsd:element name="properties">
@@ -1681,6 +1686,10 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1716,6 +1725,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6a92d384-3284-4b7a-9267-3bd72c253f16}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ae1d7975-ef6e-42df-9d49-ebdd19403660" elementFormDefault="qualified">
@@ -1778,6 +1798,23 @@
     <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0ad816ea-8460-453a-b1af-cd753e23c00d" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1906,20 +1943,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{327436CE-81CF-459D-8206-B6D3BF38F666}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9409f0e5-2b9e-47f2-90e0-3ea5ffa6bd98"/>
-    <ds:schemaRef ds:uri="ae1d7975-ef6e-42df-9d49-ebdd19403660"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{697BF653-A981-4ED3-84CB-DFE8909D8D2F}"/>
 </file>
</xml_diff>